<commit_message>
Meta-analysis using random effects model
</commit_message>
<xml_diff>
--- a/Sample_Location_Pub_year.xlsx
+++ b/Sample_Location_Pub_year.xlsx
@@ -1,35 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20356"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lkast1\Google Drive\PhD\2.Analysis\1.Quantitative synthesis\5. Data Analysis\Paper 1 - meta-averages\V3\BE-TU-Meta-analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laura\Google Drive\PhD\2.Analysis\1.Quantitative synthesis\5. Data Analysis\Paper 1 - meta-averages\V3\BE-TU-Meta-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D95A1F-762F-4E14-81CD-45EC89251D55}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43003FC2-0E6E-4F06-B623-65D328969CFD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11325" xr2:uid="{F911CA22-BBF8-4E21-B9F9-03766C57F666}"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10360" xr2:uid="{F911CA22-BBF8-4E21-B9F9-03766C57F666}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$Z$2:$AC$14</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="394" r:id="rId2"/>
-    <pivotCache cacheId="405" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId2"/>
+    <pivotCache cacheId="1" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1162" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1177" uniqueCount="57">
   <si>
     <t>Country</t>
   </si>
@@ -2906,7 +2915,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{46BBEC49-9DC0-4A13-9FF8-7BAF230B7039}" name="PivotTable39" cacheId="405" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{46BBEC49-9DC0-4A13-9FF8-7BAF230B7039}" name="PivotTable39" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="P2:S16" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField showAll="0"/>
@@ -3010,7 +3019,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2E82A4C8-C852-454A-AD7E-D055D8417193}" name="PivotTable36" cacheId="394" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2E82A4C8-C852-454A-AD7E-D055D8417193}" name="PivotTable36" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="E1:H34" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField showAll="0"/>
@@ -3491,25 +3500,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0085ACF-C466-4DBD-8EE4-EA6A7FD35ABD}">
-  <dimension ref="A1:T449"/>
+  <dimension ref="A1:AC449"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="W43" sqref="W43"/>
+      <selection activeCell="Q43" sqref="Q43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.7265625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.1796875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3523,7 +3532,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -3560,8 +3569,18 @@
       <c r="Q2" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Z2" s="5"/>
+      <c r="AA2" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC2" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -3599,8 +3618,18 @@
       <c r="S3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Z3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA3" s="8">
+        <v>3</v>
+      </c>
+      <c r="AB3" s="8"/>
+      <c r="AC3" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -3641,8 +3670,20 @@
       <c r="S4" s="3">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Z4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA4" s="8">
+        <v>2</v>
+      </c>
+      <c r="AB4" s="8">
+        <v>1</v>
+      </c>
+      <c r="AC4" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -3683,8 +3724,20 @@
       <c r="S5" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Z5" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA5" s="8">
+        <v>4</v>
+      </c>
+      <c r="AB5" s="8">
+        <v>1</v>
+      </c>
+      <c r="AC5" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -3727,8 +3780,18 @@
       <c r="S6" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Z6" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA6" s="8">
+        <v>6</v>
+      </c>
+      <c r="AB6" s="8"/>
+      <c r="AC6" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -3769,8 +3832,20 @@
       <c r="S7" s="3">
         <v>27</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Z7" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA7" s="8">
+        <v>4</v>
+      </c>
+      <c r="AB7" s="8">
+        <v>2</v>
+      </c>
+      <c r="AC7" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -3808,8 +3883,20 @@
       <c r="S8" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Z8" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA8" s="8">
+        <v>5</v>
+      </c>
+      <c r="AB8" s="8">
+        <v>2</v>
+      </c>
+      <c r="AC8" s="8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -3845,8 +3932,18 @@
       <c r="S9" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Z9" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA9" s="8">
+        <v>7</v>
+      </c>
+      <c r="AB9" s="8"/>
+      <c r="AC9" s="8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -3884,8 +3981,20 @@
       <c r="S10" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Z10" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA10" s="8">
+        <v>9</v>
+      </c>
+      <c r="AB10" s="8">
+        <v>1</v>
+      </c>
+      <c r="AC10" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -3923,8 +4032,18 @@
       <c r="S11" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Z11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA11" s="8">
+        <v>12</v>
+      </c>
+      <c r="AB11" s="8"/>
+      <c r="AC11" s="8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -3967,8 +4086,20 @@
       <c r="S12" s="3">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Z12" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA12" s="8">
+        <v>10</v>
+      </c>
+      <c r="AB12" s="8">
+        <v>3</v>
+      </c>
+      <c r="AC12" s="8">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -4004,8 +4135,20 @@
       <c r="S13" s="3">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Z13" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA13" s="8">
+        <v>26</v>
+      </c>
+      <c r="AB13" s="8">
+        <v>1</v>
+      </c>
+      <c r="AC13" s="8">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -4041,8 +4184,20 @@
       <c r="S14" s="3">
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Z14" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA14" s="8">
+        <v>54</v>
+      </c>
+      <c r="AB14" s="8">
+        <v>34</v>
+      </c>
+      <c r="AC14" s="8">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -4081,7 +4236,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -4123,7 +4278,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -4150,7 +4305,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -4177,7 +4332,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -4214,7 +4369,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>2</v>
       </c>
@@ -4254,8 +4409,16 @@
         <f>S20/187</f>
         <v>3.2085561497326207E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U20">
+        <f>1-U21</f>
+        <v>0.61971830985915499</v>
+      </c>
+      <c r="V20">
+        <f>1-V21</f>
+        <v>0.24444444444444446</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -4297,8 +4460,16 @@
         <f t="shared" ref="T21:T24" si="0">S21/187</f>
         <v>0.47058823529411764</v>
       </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U21">
+        <f>Q21/GETPIVOTDATA("Studies",$P$2,"Publication period","2010-2019")</f>
+        <v>0.38028169014084506</v>
+      </c>
+      <c r="V21">
+        <f>R21/GETPIVOTDATA("Studies",$P$2,"Publication period","Pre-2010")</f>
+        <v>0.75555555555555554</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>2</v>
       </c>
@@ -4341,7 +4512,7 @@
         <v>6.9518716577540107E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -4387,7 +4558,7 @@
         <v>6.4171122994652413E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>2</v>
       </c>
@@ -4435,7 +4606,7 @@
         <v>5.3475935828877004E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -4477,7 +4648,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -4517,7 +4688,7 @@
         <v>0.68983957219251335</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>2</v>
       </c>
@@ -4544,7 +4715,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>2</v>
       </c>
@@ -4580,7 +4751,7 @@
       <c r="R28" s="5"/>
       <c r="S28" s="5"/>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>6</v>
       </c>
@@ -4628,7 +4799,7 @@
         <v>3.7433155080213901E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>6</v>
       </c>
@@ -4671,7 +4842,7 @@
         <v>0.14438502673796791</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>5</v>
       </c>
@@ -4717,7 +4888,7 @@
         <v>1.6042780748663103E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>2</v>
       </c>
@@ -4763,7 +4934,7 @@
         <v>1.6042780748663103E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>2</v>
       </c>
@@ -4809,7 +4980,7 @@
         <v>2.6737967914438502E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>2</v>
       </c>
@@ -4857,7 +5028,7 @@
         <v>3.2085561497326207E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>7</v>
       </c>
@@ -4888,7 +5059,7 @@
         <v>3.7433155080213901E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>6</v>
       </c>
@@ -4923,7 +5094,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>2</v>
       </c>
@@ -4948,7 +5119,7 @@
         <v>0.35915492957746481</v>
       </c>
       <c r="R37" s="10">
-        <f t="shared" ref="R37:S37" si="4">R36/GETPIVOTDATA("Studies",$P$2,"Publication period","2010-2019")</f>
+        <f t="shared" ref="R37" si="4">R36/GETPIVOTDATA("Studies",$P$2,"Publication period","2010-2019")</f>
         <v>4.9295774647887321E-2</v>
       </c>
       <c r="S37" s="10">
@@ -4956,7 +5127,7 @@
         <v>0.40845070422535212</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>2</v>
       </c>
@@ -4973,7 +5144,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>6</v>
       </c>
@@ -4994,7 +5165,7 @@
       </c>
       <c r="P39" s="11"/>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>6</v>
       </c>
@@ -5014,7 +5185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>2</v>
       </c>
@@ -5034,7 +5205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>6</v>
       </c>
@@ -5054,7 +5225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>2</v>
       </c>
@@ -5074,7 +5245,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>2</v>
       </c>
@@ -5094,7 +5265,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>2</v>
       </c>
@@ -5114,7 +5285,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>2</v>
       </c>
@@ -5134,7 +5305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>5</v>
       </c>
@@ -5151,7 +5322,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>5</v>
       </c>
@@ -5171,7 +5342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>2</v>
       </c>
@@ -5191,7 +5362,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>2</v>
       </c>
@@ -5211,7 +5382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>8</v>
       </c>
@@ -5231,7 +5402,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>5</v>
       </c>
@@ -5251,7 +5422,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>2</v>
       </c>
@@ -5271,7 +5442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>6</v>
       </c>
@@ -5291,7 +5462,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>2</v>
       </c>
@@ -5311,7 +5482,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>2</v>
       </c>
@@ -5331,7 +5502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>6</v>
       </c>
@@ -5351,7 +5522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>9</v>
       </c>
@@ -5371,7 +5542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>6</v>
       </c>
@@ -5391,7 +5562,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>2</v>
       </c>
@@ -5411,7 +5582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>6</v>
       </c>
@@ -5431,7 +5602,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>5</v>
       </c>
@@ -5451,7 +5622,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>6</v>
       </c>
@@ -5471,7 +5642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>6</v>
       </c>
@@ -5491,7 +5662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>6</v>
       </c>
@@ -5499,7 +5670,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>6</v>
       </c>
@@ -5507,7 +5678,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>6</v>
       </c>
@@ -5515,7 +5686,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>2</v>
       </c>
@@ -5523,7 +5694,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>6</v>
       </c>
@@ -5531,7 +5702,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>6</v>
       </c>
@@ -5539,7 +5710,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>2</v>
       </c>
@@ -5547,7 +5718,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>10</v>
       </c>
@@ -5555,7 +5726,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>6</v>
       </c>
@@ -5563,7 +5734,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>6</v>
       </c>
@@ -5571,7 +5742,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>2</v>
       </c>
@@ -5579,7 +5750,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>2</v>
       </c>
@@ -5587,7 +5758,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>2</v>
       </c>
@@ -5595,7 +5766,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>11</v>
       </c>
@@ -5603,7 +5774,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>6</v>
       </c>
@@ -5611,7 +5782,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>6</v>
       </c>
@@ -5619,7 +5790,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>11</v>
       </c>
@@ -5627,7 +5798,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>2</v>
       </c>
@@ -5635,7 +5806,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>2</v>
       </c>
@@ -5643,7 +5814,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>2</v>
       </c>
@@ -5651,7 +5822,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>8</v>
       </c>
@@ -5659,7 +5830,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>8</v>
       </c>
@@ -5667,7 +5838,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>6</v>
       </c>
@@ -5675,7 +5846,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>6</v>
       </c>
@@ -5683,7 +5854,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>6</v>
       </c>
@@ -5691,7 +5862,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>2</v>
       </c>
@@ -5699,7 +5870,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>2</v>
       </c>
@@ -5707,7 +5878,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>6</v>
       </c>
@@ -5715,7 +5886,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>2</v>
       </c>
@@ -5723,7 +5894,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>2</v>
       </c>
@@ -5731,7 +5902,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>2</v>
       </c>
@@ -5739,7 +5910,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>2</v>
       </c>
@@ -5747,7 +5918,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>5</v>
       </c>
@@ -5755,7 +5926,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>2</v>
       </c>
@@ -5763,7 +5934,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>2</v>
       </c>
@@ -5771,7 +5942,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>2</v>
       </c>
@@ -5779,7 +5950,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>12</v>
       </c>
@@ -5787,7 +5958,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>5</v>
       </c>
@@ -5795,7 +5966,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>2</v>
       </c>
@@ -5803,7 +5974,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>2</v>
       </c>
@@ -5811,7 +5982,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>4</v>
       </c>
@@ -5819,7 +5990,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>2</v>
       </c>
@@ -5827,7 +5998,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>2</v>
       </c>
@@ -5835,7 +6006,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>2</v>
       </c>
@@ -5843,7 +6014,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>2</v>
       </c>
@@ -5851,7 +6022,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>2</v>
       </c>
@@ -5859,7 +6030,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>2</v>
       </c>
@@ -5867,7 +6038,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>2</v>
       </c>
@@ -5875,7 +6046,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>2</v>
       </c>
@@ -5883,7 +6054,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>5</v>
       </c>
@@ -5891,7 +6062,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>2</v>
       </c>
@@ -5899,7 +6070,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>5</v>
       </c>
@@ -5907,7 +6078,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>6</v>
       </c>
@@ -5915,7 +6086,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>12</v>
       </c>
@@ -5923,7 +6094,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>2</v>
       </c>
@@ -5931,7 +6102,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>6</v>
       </c>
@@ -5939,7 +6110,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>5</v>
       </c>
@@ -5947,7 +6118,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>13</v>
       </c>
@@ -5955,7 +6126,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>6</v>
       </c>
@@ -5963,7 +6134,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>10</v>
       </c>
@@ -5971,7 +6142,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>9</v>
       </c>
@@ -5979,7 +6150,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>5</v>
       </c>
@@ -5987,7 +6158,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>6</v>
       </c>
@@ -5995,7 +6166,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>6</v>
       </c>
@@ -6003,7 +6174,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>2</v>
       </c>
@@ -6011,7 +6182,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>6</v>
       </c>
@@ -6019,7 +6190,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>2</v>
       </c>
@@ -6027,7 +6198,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>6</v>
       </c>
@@ -6035,7 +6206,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>6</v>
       </c>
@@ -6043,7 +6214,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>6</v>
       </c>
@@ -6051,7 +6222,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>2</v>
       </c>
@@ -6059,7 +6230,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>14</v>
       </c>
@@ -6067,7 +6238,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>6</v>
       </c>
@@ -6075,7 +6246,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>8</v>
       </c>
@@ -6083,7 +6254,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>6</v>
       </c>
@@ -6091,7 +6262,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>6</v>
       </c>
@@ -6099,7 +6270,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>7</v>
       </c>
@@ -6107,7 +6278,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>11</v>
       </c>
@@ -6115,7 +6286,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>2</v>
       </c>
@@ -6123,7 +6294,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>2</v>
       </c>
@@ -6131,7 +6302,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>12</v>
       </c>
@@ -6139,7 +6310,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>5</v>
       </c>
@@ -6147,7 +6318,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>2</v>
       </c>
@@ -6155,7 +6326,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>6</v>
       </c>
@@ -6163,7 +6334,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>2</v>
       </c>
@@ -6171,7 +6342,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>6</v>
       </c>
@@ -6179,7 +6350,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>6</v>
       </c>
@@ -6187,7 +6358,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>6</v>
       </c>
@@ -6195,7 +6366,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>4</v>
       </c>
@@ -6203,7 +6374,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>5</v>
       </c>
@@ -6211,7 +6382,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>2</v>
       </c>
@@ -6219,7 +6390,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>6</v>
       </c>
@@ -6227,7 +6398,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>6</v>
       </c>
@@ -6235,7 +6406,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>10</v>
       </c>
@@ -6243,7 +6414,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>7</v>
       </c>
@@ -6251,7 +6422,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>6</v>
       </c>
@@ -6259,7 +6430,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>2</v>
       </c>
@@ -6267,7 +6438,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>2</v>
       </c>
@@ -6275,7 +6446,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>6</v>
       </c>
@@ -6283,7 +6454,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>2</v>
       </c>
@@ -6291,7 +6462,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>2</v>
       </c>
@@ -6299,7 +6470,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>2</v>
       </c>
@@ -6307,7 +6478,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>5</v>
       </c>
@@ -6315,7 +6486,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>6</v>
       </c>
@@ -6323,7 +6494,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>2</v>
       </c>
@@ -6331,7 +6502,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>6</v>
       </c>
@@ -6339,7 +6510,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>6</v>
       </c>
@@ -6347,7 +6518,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>6</v>
       </c>
@@ -6355,7 +6526,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>6</v>
       </c>
@@ -6363,7 +6534,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>2</v>
       </c>
@@ -6371,7 +6542,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>6</v>
       </c>
@@ -6379,7 +6550,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>2</v>
       </c>
@@ -6387,7 +6558,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>6</v>
       </c>
@@ -6395,7 +6566,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>6</v>
       </c>
@@ -6403,7 +6574,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>2</v>
       </c>
@@ -6411,7 +6582,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>6</v>
       </c>
@@ -6419,7 +6590,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>13</v>
       </c>
@@ -6427,7 +6598,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>2</v>
       </c>
@@ -6435,7 +6606,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>6</v>
       </c>
@@ -6443,7 +6614,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>2</v>
       </c>
@@ -6451,7 +6622,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>6</v>
       </c>
@@ -6459,7 +6630,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>2</v>
       </c>
@@ -6467,7 +6638,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>2</v>
       </c>
@@ -6475,7 +6646,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>2</v>
       </c>
@@ -6483,7 +6654,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>6</v>
       </c>
@@ -6491,7 +6662,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>2</v>
       </c>
@@ -6499,7 +6670,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>2</v>
       </c>
@@ -6507,7 +6678,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>6</v>
       </c>
@@ -6515,7 +6686,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>6</v>
       </c>
@@ -6523,7 +6694,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>2</v>
       </c>
@@ -6531,7 +6702,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
         <v>2</v>
       </c>
@@ -6539,7 +6710,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>2</v>
       </c>
@@ -6547,7 +6718,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
         <v>6</v>
       </c>
@@ -6555,7 +6726,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>2</v>
       </c>
@@ -6563,7 +6734,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
         <v>6</v>
       </c>
@@ -6571,7 +6742,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
         <v>10</v>
       </c>
@@ -6579,7 +6750,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
         <v>6</v>
       </c>
@@ -6587,7 +6758,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
         <v>4</v>
       </c>
@@ -6595,7 +6766,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
         <v>9</v>
       </c>
@@ -6603,7 +6774,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
         <v>6</v>
       </c>
@@ -6611,7 +6782,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
         <v>2</v>
       </c>
@@ -6619,7 +6790,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
         <v>10</v>
       </c>
@@ -6627,7 +6798,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
         <v>2</v>
       </c>
@@ -6635,7 +6806,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
         <v>2</v>
       </c>
@@ -6643,7 +6814,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
         <v>2</v>
       </c>
@@ -6651,7 +6822,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
         <v>4</v>
       </c>
@@ -6659,7 +6830,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
         <v>6</v>
       </c>
@@ -6667,7 +6838,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
         <v>2</v>
       </c>
@@ -6675,7 +6846,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
         <v>2</v>
       </c>
@@ -6683,7 +6854,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
         <v>4</v>
       </c>
@@ -6691,7 +6862,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
         <v>2</v>
       </c>
@@ -6699,7 +6870,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
         <v>6</v>
       </c>
@@ -6707,7 +6878,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
         <v>2</v>
       </c>
@@ -6715,7 +6886,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
         <v>10</v>
       </c>
@@ -6723,7 +6894,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
         <v>2</v>
       </c>
@@ -6731,7 +6902,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
         <v>6</v>
       </c>
@@ -6739,7 +6910,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
         <v>6</v>
       </c>
@@ -6747,7 +6918,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
         <v>6</v>
       </c>
@@ -6755,7 +6926,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
         <v>5</v>
       </c>
@@ -6763,7 +6934,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
         <v>2</v>
       </c>
@@ -6771,7 +6942,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
         <v>2</v>
       </c>
@@ -6779,7 +6950,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
         <v>2</v>
       </c>
@@ -6787,7 +6958,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
         <v>2</v>
       </c>
@@ -6795,7 +6966,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
         <v>2</v>
       </c>
@@ -6803,7 +6974,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
         <v>6</v>
       </c>
@@ -6811,7 +6982,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
         <v>2</v>
       </c>
@@ -6819,7 +6990,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
         <v>2</v>
       </c>
@@ -6827,7 +6998,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
         <v>8</v>
       </c>
@@ -6835,7 +7006,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
         <v>2</v>
       </c>
@@ -6843,7 +7014,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
         <v>6</v>
       </c>
@@ -6851,7 +7022,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
         <v>2</v>
       </c>
@@ -6859,7 +7030,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
         <v>2</v>
       </c>
@@ -6867,7 +7038,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
         <v>8</v>
       </c>
@@ -6875,7 +7046,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
         <v>2</v>
       </c>
@@ -6883,7 +7054,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
         <v>4</v>
       </c>
@@ -6891,7 +7062,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
         <v>2</v>
       </c>
@@ -6899,7 +7070,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
         <v>2</v>
       </c>
@@ -6907,7 +7078,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
         <v>2</v>
       </c>
@@ -6915,7 +7086,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
         <v>14</v>
       </c>
@@ -6923,7 +7094,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
         <v>6</v>
       </c>
@@ -6931,7 +7102,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
         <v>15</v>
       </c>
@@ -6939,7 +7110,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
         <v>6</v>
       </c>
@@ -6947,7 +7118,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
         <v>5</v>
       </c>
@@ -6955,7 +7126,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
         <v>5</v>
       </c>
@@ -6963,7 +7134,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
         <v>2</v>
       </c>
@@ -6971,7 +7142,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
         <v>2</v>
       </c>
@@ -6979,7 +7150,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
         <v>6</v>
       </c>
@@ -6987,7 +7158,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
         <v>6</v>
       </c>
@@ -6995,7 +7166,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A253" t="s">
         <v>6</v>
       </c>
@@ -7003,7 +7174,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A254" t="s">
         <v>2</v>
       </c>
@@ -7011,7 +7182,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
         <v>2</v>
       </c>
@@ -7019,7 +7190,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A256" t="s">
         <v>2</v>
       </c>
@@ -7027,7 +7198,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A257" t="s">
         <v>4</v>
       </c>
@@ -7035,7 +7206,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
         <v>2</v>
       </c>
@@ -7043,7 +7214,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A259" t="s">
         <v>2</v>
       </c>
@@ -7051,7 +7222,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A260" t="s">
         <v>2</v>
       </c>
@@ -7059,7 +7230,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A261" t="s">
         <v>2</v>
       </c>
@@ -7067,7 +7238,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A262" t="s">
         <v>2</v>
       </c>
@@ -7075,7 +7246,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A263" t="s">
         <v>2</v>
       </c>
@@ -7083,7 +7254,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
         <v>15</v>
       </c>
@@ -7091,7 +7262,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A265" t="s">
         <v>2</v>
       </c>
@@ -7099,7 +7270,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A266" t="s">
         <v>6</v>
       </c>
@@ -7107,7 +7278,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A267" t="s">
         <v>6</v>
       </c>
@@ -7115,7 +7286,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A268" t="s">
         <v>2</v>
       </c>
@@ -7123,7 +7294,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A269" t="s">
         <v>8</v>
       </c>
@@ -7131,7 +7302,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A270" t="s">
         <v>2</v>
       </c>
@@ -7139,7 +7310,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A271" t="s">
         <v>2</v>
       </c>
@@ -7147,7 +7318,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A272" t="s">
         <v>3</v>
       </c>
@@ -7155,7 +7326,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A273" t="s">
         <v>2</v>
       </c>
@@ -7163,7 +7334,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A274" t="s">
         <v>2</v>
       </c>
@@ -7171,7 +7342,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A275" t="s">
         <v>2</v>
       </c>
@@ -7179,7 +7350,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A276" t="s">
         <v>5</v>
       </c>
@@ -7187,7 +7358,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A277" t="s">
         <v>2</v>
       </c>
@@ -7195,7 +7366,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A278" t="s">
         <v>5</v>
       </c>
@@ -7203,7 +7374,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A279" t="s">
         <v>5</v>
       </c>
@@ -7211,7 +7382,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A280" t="s">
         <v>2</v>
       </c>
@@ -7219,7 +7390,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A281" t="s">
         <v>6</v>
       </c>
@@ -7227,7 +7398,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A282" t="s">
         <v>6</v>
       </c>
@@ -7235,7 +7406,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A283" t="s">
         <v>16</v>
       </c>
@@ -7243,7 +7414,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A284" t="s">
         <v>2</v>
       </c>
@@ -7251,7 +7422,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A285" t="s">
         <v>2</v>
       </c>
@@ -7259,7 +7430,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A286" t="s">
         <v>2</v>
       </c>
@@ -7267,7 +7438,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A287" t="s">
         <v>6</v>
       </c>
@@ -7275,7 +7446,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A288" t="s">
         <v>16</v>
       </c>
@@ -7283,7 +7454,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A289" t="s">
         <v>2</v>
       </c>
@@ -7291,7 +7462,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A290" t="s">
         <v>2</v>
       </c>
@@ -7299,7 +7470,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A291" t="s">
         <v>2</v>
       </c>
@@ -7307,7 +7478,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A292" t="s">
         <v>2</v>
       </c>
@@ -7315,7 +7486,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A293" t="s">
         <v>6</v>
       </c>
@@ -7323,7 +7494,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A294" t="s">
         <v>6</v>
       </c>
@@ -7331,7 +7502,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="295" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A295" t="s">
         <v>2</v>
       </c>
@@ -7339,7 +7510,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="296" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A296" t="s">
         <v>17</v>
       </c>
@@ -7347,7 +7518,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="297" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A297" t="s">
         <v>18</v>
       </c>
@@ -7355,7 +7526,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="298" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A298" t="s">
         <v>2</v>
       </c>
@@ -7363,7 +7534,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="299" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A299" t="s">
         <v>2</v>
       </c>
@@ -7371,7 +7542,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="300" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A300" t="s">
         <v>19</v>
       </c>
@@ -7379,7 +7550,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="301" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A301" t="s">
         <v>20</v>
       </c>
@@ -7387,7 +7558,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="302" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A302" t="s">
         <v>2</v>
       </c>
@@ -7395,7 +7566,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="303" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A303" t="s">
         <v>16</v>
       </c>
@@ -7403,7 +7574,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="304" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A304" t="s">
         <v>2</v>
       </c>
@@ -7411,7 +7582,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="305" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A305" t="s">
         <v>2</v>
       </c>
@@ -7419,7 +7590,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="306" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A306" t="s">
         <v>2</v>
       </c>
@@ -7427,7 +7598,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="307" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A307" t="s">
         <v>5</v>
       </c>
@@ -7435,7 +7606,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="308" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A308" t="s">
         <v>6</v>
       </c>
@@ -7443,7 +7614,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="309" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A309" t="s">
         <v>2</v>
       </c>
@@ -7451,7 +7622,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="310" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A310" t="s">
         <v>2</v>
       </c>
@@ -7459,7 +7630,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="311" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A311" t="s">
         <v>2</v>
       </c>
@@ -7467,7 +7638,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="312" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A312" t="s">
         <v>2</v>
       </c>
@@ -7475,7 +7646,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="313" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A313" t="s">
         <v>2</v>
       </c>
@@ -7483,7 +7654,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="314" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A314" t="s">
         <v>10</v>
       </c>
@@ -7491,7 +7662,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="315" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A315" t="s">
         <v>2</v>
       </c>
@@ -7499,7 +7670,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="316" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A316" t="s">
         <v>5</v>
       </c>
@@ -7507,7 +7678,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="317" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A317" t="s">
         <v>6</v>
       </c>
@@ -7515,7 +7686,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="318" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A318" t="s">
         <v>2</v>
       </c>
@@ -7523,7 +7694,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="319" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A319" t="s">
         <v>5</v>
       </c>
@@ -7531,7 +7702,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="320" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A320" t="s">
         <v>14</v>
       </c>
@@ -7539,7 +7710,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="321" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A321" t="s">
         <v>2</v>
       </c>
@@ -7547,7 +7718,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="322" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A322" t="s">
         <v>2</v>
       </c>
@@ -7555,7 +7726,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="323" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A323" t="s">
         <v>5</v>
       </c>
@@ -7563,7 +7734,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="324" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A324" t="s">
         <v>2</v>
       </c>
@@ -7571,7 +7742,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="325" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A325" t="s">
         <v>6</v>
       </c>
@@ -7579,7 +7750,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="326" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A326" t="s">
         <v>6</v>
       </c>
@@ -7587,7 +7758,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="327" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A327" t="s">
         <v>2</v>
       </c>
@@ -7595,7 +7766,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="328" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A328" t="s">
         <v>2</v>
       </c>
@@ -7603,7 +7774,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="329" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A329" t="s">
         <v>6</v>
       </c>
@@ -7611,7 +7782,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="330" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A330" t="s">
         <v>6</v>
       </c>
@@ -7619,7 +7790,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="331" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A331" t="s">
         <v>2</v>
       </c>
@@ -7627,7 +7798,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="332" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A332" t="s">
         <v>6</v>
       </c>
@@ -7635,7 +7806,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="333" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A333" t="s">
         <v>6</v>
       </c>
@@ -7643,7 +7814,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="334" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A334" t="s">
         <v>6</v>
       </c>
@@ -7651,7 +7822,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="335" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A335" t="s">
         <v>5</v>
       </c>
@@ -7659,7 +7830,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="336" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A336" t="s">
         <v>2</v>
       </c>
@@ -7667,7 +7838,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="337" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A337" t="s">
         <v>2</v>
       </c>
@@ -7675,7 +7846,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="338" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A338" t="s">
         <v>9</v>
       </c>
@@ -7683,7 +7854,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="339" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A339" t="s">
         <v>2</v>
       </c>
@@ -7691,7 +7862,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="340" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A340" t="s">
         <v>2</v>
       </c>
@@ -7699,7 +7870,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="341" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A341" t="s">
         <v>2</v>
       </c>
@@ -7707,7 +7878,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="342" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A342" t="s">
         <v>6</v>
       </c>
@@ -7715,7 +7886,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="343" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A343" t="s">
         <v>2</v>
       </c>
@@ -7723,7 +7894,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="344" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A344" t="s">
         <v>6</v>
       </c>
@@ -7731,7 +7902,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="345" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A345" t="s">
         <v>2</v>
       </c>
@@ -7739,7 +7910,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="346" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A346" t="s">
         <v>2</v>
       </c>
@@ -7747,7 +7918,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="347" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A347" t="s">
         <v>6</v>
       </c>
@@ -7755,7 +7926,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="348" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A348" t="s">
         <v>6</v>
       </c>
@@ -7763,7 +7934,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="349" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A349" t="s">
         <v>2</v>
       </c>
@@ -7771,7 +7942,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="350" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A350" t="s">
         <v>2</v>
       </c>
@@ -7779,7 +7950,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="351" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A351" t="s">
         <v>6</v>
       </c>
@@ -7787,7 +7958,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="352" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A352" t="s">
         <v>6</v>
       </c>
@@ -7795,7 +7966,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="353" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A353" t="s">
         <v>6</v>
       </c>
@@ -7803,7 +7974,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="354" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A354" t="s">
         <v>6</v>
       </c>
@@ -7811,7 +7982,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="355" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A355" t="s">
         <v>2</v>
       </c>
@@ -7819,7 +7990,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="356" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A356" t="s">
         <v>2</v>
       </c>
@@ -7827,7 +7998,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="357" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A357" t="s">
         <v>4</v>
       </c>
@@ -7835,7 +8006,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="358" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A358" t="s">
         <v>2</v>
       </c>
@@ -7843,7 +8014,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="359" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A359" t="s">
         <v>5</v>
       </c>
@@ -7851,7 +8022,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="360" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A360" t="s">
         <v>2</v>
       </c>
@@ -7859,7 +8030,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="361" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A361" t="s">
         <v>2</v>
       </c>
@@ -7867,7 +8038,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="362" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A362" t="s">
         <v>2</v>
       </c>
@@ -7875,7 +8046,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="363" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A363" t="s">
         <v>2</v>
       </c>
@@ -7883,7 +8054,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="364" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A364" t="s">
         <v>2</v>
       </c>
@@ -7891,7 +8062,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="365" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A365" t="s">
         <v>2</v>
       </c>
@@ -7899,7 +8070,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="366" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A366" t="s">
         <v>2</v>
       </c>
@@ -7907,7 +8078,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="367" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A367" t="s">
         <v>2</v>
       </c>
@@ -7915,7 +8086,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="368" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A368" t="s">
         <v>2</v>
       </c>
@@ -7923,7 +8094,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="369" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A369" t="s">
         <v>2</v>
       </c>
@@ -7931,7 +8102,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="370" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A370" t="s">
         <v>4</v>
       </c>
@@ -7939,7 +8110,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="371" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A371" t="s">
         <v>2</v>
       </c>
@@ -7947,7 +8118,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="372" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A372" t="s">
         <v>4</v>
       </c>
@@ -7955,7 +8126,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="373" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A373" t="s">
         <v>2</v>
       </c>
@@ -7963,7 +8134,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="374" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A374" t="s">
         <v>2</v>
       </c>
@@ -7971,7 +8142,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="375" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A375" t="s">
         <v>11</v>
       </c>
@@ -7979,7 +8150,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="376" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A376" t="s">
         <v>2</v>
       </c>
@@ -7987,7 +8158,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="377" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A377" t="s">
         <v>2</v>
       </c>
@@ -7995,7 +8166,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="378" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A378" t="s">
         <v>2</v>
       </c>
@@ -8003,7 +8174,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="379" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A379" t="s">
         <v>2</v>
       </c>
@@ -8011,7 +8182,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="380" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A380" t="s">
         <v>9</v>
       </c>
@@ -8019,7 +8190,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="381" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A381" t="s">
         <v>2</v>
       </c>
@@ -8027,7 +8198,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="382" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A382" t="s">
         <v>4</v>
       </c>
@@ -8035,7 +8206,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="383" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A383" t="s">
         <v>2</v>
       </c>
@@ -8043,7 +8214,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="384" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A384" t="s">
         <v>3</v>
       </c>
@@ -8051,7 +8222,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="385" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A385" t="s">
         <v>2</v>
       </c>
@@ -8059,7 +8230,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="386" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A386" t="s">
         <v>14</v>
       </c>
@@ -8067,7 +8238,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="387" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A387" t="s">
         <v>6</v>
       </c>
@@ -8075,7 +8246,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="388" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A388" t="s">
         <v>6</v>
       </c>
@@ -8083,7 +8254,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="389" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A389" t="s">
         <v>5</v>
       </c>
@@ -8091,7 +8262,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="390" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A390" t="s">
         <v>3</v>
       </c>
@@ -8099,7 +8270,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="391" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A391" t="s">
         <v>2</v>
       </c>
@@ -8107,7 +8278,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="392" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A392" t="s">
         <v>2</v>
       </c>
@@ -8115,7 +8286,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="393" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A393" t="s">
         <v>2</v>
       </c>
@@ -8123,7 +8294,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="394" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A394" t="s">
         <v>2</v>
       </c>
@@ -8131,7 +8302,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="395" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A395" t="s">
         <v>8</v>
       </c>
@@ -8139,7 +8310,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="396" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A396" t="s">
         <v>2</v>
       </c>
@@ -8147,7 +8318,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="397" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A397" t="s">
         <v>2</v>
       </c>
@@ -8155,7 +8326,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="398" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A398" t="s">
         <v>2</v>
       </c>
@@ -8163,7 +8334,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="399" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A399" t="s">
         <v>2</v>
       </c>
@@ -8171,7 +8342,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="400" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A400" t="s">
         <v>2</v>
       </c>
@@ -8179,7 +8350,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="401" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A401" t="s">
         <v>2</v>
       </c>
@@ -8187,7 +8358,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="402" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A402" t="s">
         <v>2</v>
       </c>
@@ -8195,7 +8366,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="403" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A403" t="s">
         <v>16</v>
       </c>
@@ -8203,7 +8374,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="404" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A404" t="s">
         <v>6</v>
       </c>
@@ -8211,7 +8382,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="405" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A405" t="s">
         <v>2</v>
       </c>
@@ -8219,7 +8390,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="406" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A406" t="s">
         <v>5</v>
       </c>
@@ -8227,7 +8398,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="407" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A407" t="s">
         <v>2</v>
       </c>
@@ -8235,7 +8406,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="408" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A408" t="s">
         <v>2</v>
       </c>
@@ -8243,7 +8414,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="409" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A409" t="s">
         <v>6</v>
       </c>
@@ -8251,7 +8422,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="410" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A410" t="s">
         <v>2</v>
       </c>
@@ -8259,7 +8430,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="411" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A411" t="s">
         <v>2</v>
       </c>
@@ -8267,7 +8438,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="412" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A412" t="s">
         <v>2</v>
       </c>
@@ -8275,7 +8446,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="413" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A413" t="s">
         <v>6</v>
       </c>
@@ -8283,7 +8454,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="414" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A414" t="s">
         <v>2</v>
       </c>
@@ -8291,7 +8462,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="415" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A415" t="s">
         <v>2</v>
       </c>
@@ -8299,7 +8470,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="416" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A416" t="s">
         <v>2</v>
       </c>
@@ -8307,7 +8478,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="417" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A417" t="s">
         <v>2</v>
       </c>
@@ -8315,7 +8486,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="418" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A418" t="s">
         <v>5</v>
       </c>
@@ -8323,7 +8494,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="419" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A419" t="s">
         <v>2</v>
       </c>
@@ -8331,7 +8502,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="420" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A420" t="s">
         <v>21</v>
       </c>
@@ -8339,7 +8510,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="421" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A421" t="s">
         <v>2</v>
       </c>
@@ -8347,7 +8518,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="422" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A422" t="s">
         <v>2</v>
       </c>
@@ -8355,7 +8526,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="423" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A423" t="s">
         <v>2</v>
       </c>
@@ -8363,7 +8534,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="424" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A424" t="s">
         <v>8</v>
       </c>
@@ -8371,7 +8542,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="425" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A425" t="s">
         <v>4</v>
       </c>
@@ -8379,7 +8550,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="426" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A426" t="s">
         <v>2</v>
       </c>
@@ -8387,7 +8558,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="427" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A427" t="s">
         <v>2</v>
       </c>
@@ -8395,7 +8566,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="428" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A428" t="s">
         <v>2</v>
       </c>
@@ -8403,7 +8574,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="429" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A429" t="s">
         <v>2</v>
       </c>
@@ -8411,7 +8582,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="430" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A430" t="s">
         <v>2</v>
       </c>
@@ -8419,7 +8590,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="431" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A431" t="s">
         <v>2</v>
       </c>
@@ -8427,7 +8598,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="432" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A432" t="s">
         <v>2</v>
       </c>
@@ -8435,7 +8606,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="433" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A433" t="s">
         <v>2</v>
       </c>
@@ -8443,7 +8614,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="434" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A434" t="s">
         <v>2</v>
       </c>
@@ -8451,7 +8622,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="435" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A435" t="s">
         <v>17</v>
       </c>
@@ -8459,7 +8630,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="436" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A436" t="s">
         <v>2</v>
       </c>
@@ -8467,7 +8638,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="437" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A437" t="s">
         <v>6</v>
       </c>
@@ -8475,7 +8646,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="438" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A438" t="s">
         <v>10</v>
       </c>
@@ -8483,7 +8654,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="439" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A439" t="s">
         <v>2</v>
       </c>
@@ -8491,7 +8662,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="440" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A440" t="s">
         <v>6</v>
       </c>
@@ -8499,7 +8670,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="441" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A441" t="s">
         <v>2</v>
       </c>
@@ -8507,7 +8678,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="442" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A442" t="s">
         <v>2</v>
       </c>
@@ -8515,7 +8686,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="443" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A443" t="s">
         <v>2</v>
       </c>
@@ -8523,7 +8694,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="444" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A444" t="s">
         <v>2</v>
       </c>
@@ -8531,7 +8702,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="445" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A445" t="s">
         <v>2</v>
       </c>
@@ -8539,7 +8710,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="446" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A446" t="s">
         <v>2</v>
       </c>
@@ -8547,7 +8718,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="447" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A447" t="s">
         <v>2</v>
       </c>
@@ -8555,7 +8726,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="448" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A448" t="s">
         <v>4</v>
       </c>
@@ -8563,7 +8734,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="449" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A449" t="s">
         <v>8</v>
       </c>
@@ -8572,6 +8743,11 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="Z2:AC14" xr:uid="{71EEEF02-90EA-405F-B9CD-25BB43AAA391}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="Z3:AC14">
+      <sortCondition ref="AC2:AC14"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
 </worksheet>

</xml_diff>